<commit_message>
initial parameters before filtering stored in excel file
</commit_message>
<xml_diff>
--- a/Results-Generation/subj5/results_Alpha.xlsx
+++ b/Results-Generation/subj5/results_Alpha.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Layers Number</t>
   </si>
@@ -77,9 +77,6 @@
   </si>
   <si>
     <t>Noise</t>
-  </si>
-  <si>
-    <t>movehead</t>
   </si>
 </sst>
 </file>
@@ -437,7 +434,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -508,71 +505,6 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
-      <c r="A2">
-        <v>6</v>
-      </c>
-      <c r="B2">
-        <v>20</v>
-      </c>
-      <c r="C2">
-        <v>20</v>
-      </c>
-      <c r="D2">
-        <v>20</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>2.5</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>0.5</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>15</v>
-      </c>
-      <c r="K2">
-        <v>10</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>0.01</v>
-      </c>
-      <c r="P2">
-        <v>0.01</v>
-      </c>
-      <c r="Q2">
-        <v>-1.449764027933893</v>
-      </c>
-      <c r="R2">
-        <v>3.344083949444509</v>
-      </c>
-      <c r="S2">
-        <v>2.204190255890288</v>
-      </c>
-      <c r="T2">
-        <v>4</v>
-      </c>
-      <c r="U2" t="s">
-        <v>21</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>